<commit_message>
overwrite ctu_update_last into main
</commit_message>
<xml_diff>
--- a/Data/customers.xlsx
+++ b/Data/customers.xlsx
@@ -1269,8 +1269,8 @@
     <x:row r="476" ht="14.25" customHeight="1" x14ac:dyDescent="0.3"/>
   </x:sheetData>
   <x:hyperlinks>
-    <x:hyperlink ref="K2" r:id="rId9"/>
-    <x:hyperlink ref="K3" r:id="rId10"/>
+    <x:hyperlink ref="K2" r:id="rId11"/>
+    <x:hyperlink ref="K3" r:id="rId12"/>
   </x:hyperlinks>
   <x:printOptions horizontalCentered="0" verticalCentered="0" headings="0" gridLines="0"/>
   <x:pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>

</xml_diff>